<commit_message>
phutn tạo thêm các controller
</commit_message>
<xml_diff>
--- a/C500Hemis/TaiLieu/BangHemis.xlsx
+++ b/C500Hemis/TaiLieu/BangHemis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lap trinh may tinh\Code\C500Hemis\C500Hemis\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBF872F-E658-43FD-85B7-BA3694382A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52245840-5D4A-4950-AE9B-BF0843249083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tạo controller-B9" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="381">
   <si>
     <t>tbHoatDongTaiChinh</t>
   </si>
@@ -922,15 +922,9 @@
     <t>Nhóm 8</t>
   </si>
   <si>
-    <t>Thiếu 2 bảng</t>
-  </si>
-  <si>
     <t>Ghi chú</t>
   </si>
   <si>
-    <t>mới 2/3 bảng</t>
-  </si>
-  <si>
     <t>Điểm</t>
   </si>
   <si>
@@ -1190,6 +1184,9 @@
   </si>
   <si>
     <t>Đổi tối đa</t>
+  </si>
+  <si>
+    <t>Giao diện đẹp</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1336,6 +1333,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1620,7 +1627,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -1644,10 +1651,10 @@
         <v>282</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -1663,6 +1670,9 @@
       <c r="D2" s="6">
         <v>10</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
@@ -1677,9 +1687,6 @@
       <c r="D3" s="6">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
@@ -1692,7 +1699,7 @@
         <v>286</v>
       </c>
       <c r="D4" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
@@ -1706,7 +1713,7 @@
         <v>287</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
@@ -1720,7 +1727,7 @@
         <v>288</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.5">
@@ -1734,7 +1741,7 @@
         <v>289</v>
       </c>
       <c r="D7" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.5">
@@ -1750,6 +1757,9 @@
       <c r="D8" s="6">
         <v>10</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
@@ -1762,10 +1772,7 @@
         <v>291</v>
       </c>
       <c r="D9" s="22">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>294</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
@@ -1778,25 +1785,25 @@
       <c r="C10" s="21"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A11" s="1">
+    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="24">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="A12" s="1">
+      <c r="D11" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="24">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="27">
         <v>0</v>
       </c>
     </row>
@@ -1815,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -1845,7 +1852,7 @@
         <v>247</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
@@ -1861,25 +1868,25 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>297</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>299</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>269</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.5">
@@ -6506,7 +6513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D23458-106E-45B1-B4B0-490116DEE107}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -6531,22 +6538,22 @@
         <v>246</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>378</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>379</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
@@ -8453,10 +8460,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -9188,18 +9195,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" t="s">
         <v>374</v>
-      </c>
-      <c r="B1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C1" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -9210,7 +9217,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -9243,7 +9250,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -9265,7 +9272,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -9276,7 +9283,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -9287,7 +9294,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -9298,7 +9305,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -9320,7 +9327,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -9331,7 +9338,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -9353,7 +9360,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -9364,7 +9371,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -9397,7 +9404,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -9408,7 +9415,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -9419,7 +9426,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -9430,7 +9437,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -9441,7 +9448,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -9452,7 +9459,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -9463,7 +9470,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -9474,7 +9481,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -9485,7 +9492,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -9573,7 +9580,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -9584,7 +9591,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B37">
         <v>5</v>
@@ -9595,7 +9602,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B38">
         <v>5</v>
@@ -9606,7 +9613,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B39">
         <v>5</v>
@@ -9782,7 +9789,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B55">
         <v>5</v>
@@ -9793,7 +9800,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -9804,7 +9811,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B57">
         <v>5</v>
@@ -9826,7 +9833,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B59">
         <v>6</v>
@@ -9837,7 +9844,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B60">
         <v>6</v>
@@ -9881,7 +9888,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B64">
         <v>6</v>
@@ -9892,7 +9899,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B65">
         <v>6</v>
@@ -10024,7 +10031,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B77">
         <v>7</v>
@@ -10035,7 +10042,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B78">
         <v>7</v>
@@ -10046,7 +10053,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B79">
         <v>7</v>
@@ -10079,7 +10086,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B82">
         <v>7</v>
@@ -10090,7 +10097,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B83">
         <v>7</v>
@@ -10101,7 +10108,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B84">
         <v>7</v>
@@ -10112,7 +10119,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B85">
         <v>7</v>
@@ -10123,7 +10130,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B86">
         <v>7</v>
@@ -10134,7 +10141,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B87">
         <v>7</v>
@@ -10145,7 +10152,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B88">
         <v>8</v>
@@ -10200,7 +10207,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B93">
         <v>8</v>
@@ -10211,7 +10218,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B94">
         <v>8</v>
@@ -10222,7 +10229,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B95">
         <v>8</v>
@@ -10233,7 +10240,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B96">
         <v>8</v>
@@ -10244,7 +10251,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B97">
         <v>8</v>
@@ -10398,7 +10405,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B111">
         <v>9</v>
@@ -10409,7 +10416,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B112">
         <v>9</v>
@@ -10442,7 +10449,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B115">
         <v>9</v>
@@ -10453,7 +10460,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B116">
         <v>9</v>
@@ -10464,7 +10471,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B117">
         <v>9</v>
@@ -10475,7 +10482,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B118">
         <v>9</v>
@@ -10486,7 +10493,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B119">
         <v>10</v>
@@ -10508,7 +10515,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B121">
         <v>10</v>
@@ -10519,7 +10526,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B122">
         <v>10</v>
@@ -10629,7 +10636,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B132">
         <v>11</v>
@@ -10640,7 +10647,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B133">
         <v>11</v>
@@ -10695,7 +10702,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B138">
         <v>14</v>
@@ -10706,7 +10713,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B139">
         <v>14</v>
@@ -10717,7 +10724,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B140">
         <v>15</v>
@@ -10761,7 +10768,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B144">
         <v>16</v>
@@ -10783,7 +10790,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B146">
         <v>18</v>
@@ -10794,7 +10801,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B147">
         <v>19</v>
@@ -10816,7 +10823,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B149">
         <v>19</v>
@@ -10838,7 +10845,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B151">
         <v>20</v>
@@ -10860,7 +10867,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B153">
         <v>21</v>
@@ -10893,7 +10900,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B156">
         <v>23</v>
@@ -10904,7 +10911,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B157">
         <v>23</v>
@@ -10948,7 +10955,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B161">
         <v>25</v>
@@ -10970,7 +10977,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B163">
         <v>27</v>
@@ -10981,7 +10988,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B164">
         <v>30</v>
@@ -11014,7 +11021,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B167">
         <v>36</v>

</xml_diff>

<commit_message>
phutn update controller NTD va VB
</commit_message>
<xml_diff>
--- a/C500Hemis/TaiLieu/BangHemis.xlsx
+++ b/C500Hemis/TaiLieu/BangHemis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lap trinh may tinh\Code\C500Hemis\C500Hemis\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52245840-5D4A-4950-AE9B-BF0843249083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA35BD4-4733-4E95-85D1-C7FF0F057FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tạo controller-B9" sheetId="2" r:id="rId1"/>
@@ -1325,15 +1325,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1343,6 +1334,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1768,10 +1768,10 @@
       <c r="B9" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="26">
         <v>8</v>
       </c>
     </row>
@@ -1782,28 +1782,28 @@
       <c r="B10" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="24">
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+    </row>
+    <row r="11" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="21">
         <v>8</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="D11" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="24">
+      <c r="D11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="21">
         <v>9</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="24">
         <v>0</v>
       </c>
     </row>
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -1842,31 +1842,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="27" t="s">
         <v>375</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="15" t="s">
         <v>293</v>
       </c>
@@ -9187,11 +9187,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AF3660-7BB6-4B35-A2B5-A126CAAF0875}">
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
phutn cập nhật phần Home
</commit_message>
<xml_diff>
--- a/C500Hemis/TaiLieu/BangHemis.xlsx
+++ b/C500Hemis/TaiLieu/BangHemis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lap trinh may tinh\Code\C500Hemis\C500Hemis\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA35BD4-4733-4E95-85D1-C7FF0F057FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB5EDA-E707-416C-8BE2-DA8991E179AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Đăng ký thi giữa phần'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DemTruong!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Triển khai các controller'!$A$2:$C$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1627,7 +1628,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -1822,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J234"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A206" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B226" sqref="B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -6513,8 +6514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D23458-106E-45B1-B4B0-490116DEE107}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.5"/>
@@ -8449,8 +8450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E7C508-4C5E-48AF-9FA8-F826894616CF}">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9187,13 +9188,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05AF3660-7BB6-4B35-A2B5-A126CAAF0875}">
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
     <col min="2" max="2" width="9.796875" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -9211,10 +9212,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -9222,43 +9223,43 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>339</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>338</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>302</v>
+        <v>363</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -9266,32 +9267,32 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>336</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>350</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -9299,10 +9300,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -9310,76 +9311,76 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>351</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>307</v>
+        <v>368</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>308</v>
+        <v>369</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>345</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>344</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>310</v>
+        <v>343</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -9387,10 +9388,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>306</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -9398,10 +9399,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>124</v>
+        <v>335</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -9409,13 +9410,13 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>311</v>
+        <v>362</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -9431,10 +9432,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>313</v>
+        <v>354</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -9442,18 +9443,18 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
       <c r="B23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -9464,10 +9465,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -9475,21 +9476,21 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>317</v>
+        <v>353</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -9497,10 +9498,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="B28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -9508,40 +9509,40 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>360</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>236</v>
+        <v>346</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>371</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -9552,21 +9553,21 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>329</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>304</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -9574,7 +9575,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>319</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -9585,43 +9586,43 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>322</v>
+        <v>347</v>
       </c>
       <c r="B38">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -9629,10 +9630,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -9640,32 +9641,32 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>316</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>315</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -9673,32 +9674,32 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>355</v>
       </c>
       <c r="B44">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>364</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>314</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -9706,21 +9707,21 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>358</v>
       </c>
       <c r="B47">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -9728,43 +9729,43 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>342</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>43</v>
+        <v>341</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="B51">
         <v>5</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>365</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -9772,7 +9773,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>325</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -9783,7 +9784,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>0</v>
+        <v>324</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -9794,10 +9795,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -9805,32 +9806,32 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="B56">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="B57">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>308</v>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -9838,10 +9839,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -9849,128 +9850,128 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="B60">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>367</v>
       </c>
       <c r="B61">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>233</v>
+        <v>349</v>
       </c>
       <c r="B62">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>46</v>
+        <v>328</v>
       </c>
       <c r="B63">
         <v>6</v>
       </c>
       <c r="C63">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>329</v>
+        <v>370</v>
       </c>
       <c r="B64">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>334</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>361</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>240</v>
+        <v>366</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>178</v>
+        <v>310</v>
       </c>
       <c r="B69">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>173</v>
+        <v>309</v>
       </c>
       <c r="B70">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>327</v>
       </c>
       <c r="B71">
         <v>6</v>
@@ -9981,32 +9982,32 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>190</v>
+        <v>356</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>307</v>
       </c>
       <c r="B73">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>237</v>
+        <v>49</v>
       </c>
       <c r="B74">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -10014,10 +10015,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B75">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -10025,10 +10026,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B76">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76">
         <v>2</v>
@@ -10036,10 +10037,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>331</v>
+        <v>133</v>
       </c>
       <c r="B77">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -10047,21 +10048,21 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>332</v>
+        <v>104</v>
       </c>
       <c r="B78">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>333</v>
+        <v>74</v>
       </c>
       <c r="B79">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -10069,21 +10070,21 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="B80">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -10091,10 +10092,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>334</v>
+        <v>225</v>
       </c>
       <c r="B82">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -10102,10 +10103,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>335</v>
+        <v>195</v>
       </c>
       <c r="B83">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -10113,21 +10114,21 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>336</v>
+        <v>91</v>
       </c>
       <c r="B84">
         <v>7</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>337</v>
+        <v>130</v>
       </c>
       <c r="B85">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -10135,109 +10136,109 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>338</v>
+        <v>224</v>
       </c>
       <c r="B86">
+        <v>23</v>
+      </c>
+      <c r="C86">
         <v>7</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="B87">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>340</v>
+        <v>216</v>
       </c>
       <c r="B88">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="B89">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B90">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B91">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>229</v>
+        <v>170</v>
       </c>
       <c r="B92">
         <v>8</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>341</v>
+        <v>166</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>342</v>
+        <v>20</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C94">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>343</v>
+        <v>161</v>
       </c>
       <c r="B95">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -10245,43 +10246,43 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>344</v>
+        <v>88</v>
       </c>
       <c r="B96">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>345</v>
+        <v>10</v>
       </c>
       <c r="B97">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="B98">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="B99">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -10289,10 +10290,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B100">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -10300,109 +10301,109 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>228</v>
+        <v>65</v>
       </c>
       <c r="B101">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C101">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>208</v>
+        <v>62</v>
       </c>
       <c r="B102">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="B103">
         <v>8</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B104">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>155</v>
       </c>
       <c r="B105">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B106">
         <v>8</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="B107">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B108">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="B109">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>149</v>
+        <v>236</v>
       </c>
       <c r="B110">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -10410,10 +10411,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>346</v>
+        <v>82</v>
       </c>
       <c r="B111">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -10421,21 +10422,21 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>347</v>
+        <v>121</v>
       </c>
       <c r="B112">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="B113">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -10443,21 +10444,21 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="B114">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>348</v>
+        <v>232</v>
       </c>
       <c r="B115">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -10465,21 +10466,21 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>349</v>
+        <v>43</v>
       </c>
       <c r="B116">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>350</v>
+        <v>208</v>
       </c>
       <c r="B117">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -10487,10 +10488,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>351</v>
+        <v>228</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -10498,32 +10499,32 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>352</v>
+        <v>59</v>
       </c>
       <c r="B119">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C119">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>183</v>
       </c>
       <c r="B120">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C120">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>353</v>
+        <v>11</v>
       </c>
       <c r="B121">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -10531,10 +10532,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>354</v>
+        <v>7</v>
       </c>
       <c r="B122">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -10542,10 +10543,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B123">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -10553,10 +10554,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B124">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C124">
         <v>3</v>
@@ -10575,7 +10576,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>215</v>
       </c>
       <c r="B126">
         <v>10</v>
@@ -10586,21 +10587,21 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="B127">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="B128">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -10608,65 +10609,65 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>223</v>
+        <v>0</v>
       </c>
       <c r="B129">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C129">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="B130">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C130">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B131">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C131">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>355</v>
+        <v>115</v>
       </c>
       <c r="B132">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>356</v>
+        <v>211</v>
       </c>
       <c r="B133">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="B134">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -10674,10 +10675,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
       <c r="B135">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -10685,10 +10686,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="B136">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -10696,10 +10697,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>244</v>
+        <v>29</v>
       </c>
       <c r="B137">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C137">
         <v>1</v>
@@ -10707,32 +10708,32 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>357</v>
+        <v>203</v>
       </c>
       <c r="B138">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>358</v>
+        <v>37</v>
       </c>
       <c r="B139">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C139">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>359</v>
+        <v>198</v>
       </c>
       <c r="B140">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C140">
         <v>3</v>
@@ -10740,10 +10741,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="B141">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -10751,76 +10752,76 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>33</v>
+        <v>194</v>
       </c>
       <c r="B142">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C142">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B143">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C143">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>360</v>
+        <v>112</v>
       </c>
       <c r="B144">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="B145">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C145">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>361</v>
+        <v>108</v>
       </c>
       <c r="B146">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>362</v>
+        <v>32</v>
       </c>
       <c r="B147">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C147">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>140</v>
+        <v>56</v>
       </c>
       <c r="B148">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -10828,21 +10829,21 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>363</v>
+        <v>33</v>
       </c>
       <c r="B149">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B150">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C150">
         <v>3</v>
@@ -10850,21 +10851,21 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>364</v>
+        <v>199</v>
       </c>
       <c r="B151">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C151">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="B152">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -10872,10 +10873,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>365</v>
+        <v>186</v>
       </c>
       <c r="B153">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -10883,10 +10884,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>29</v>
+        <v>182</v>
       </c>
       <c r="B154">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -10894,46 +10895,46 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="B155">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C155">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>366</v>
+        <v>52</v>
       </c>
       <c r="B156">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C156">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>367</v>
+        <v>18</v>
       </c>
       <c r="B157">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C157">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B158">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C158">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
@@ -10949,65 +10950,65 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B160">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C160">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>368</v>
+        <v>24</v>
       </c>
       <c r="B161">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C161">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>164</v>
+        <v>241</v>
       </c>
       <c r="B162">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C162">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>369</v>
+        <v>237</v>
       </c>
       <c r="B163">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>370</v>
+        <v>173</v>
       </c>
       <c r="B164">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C164">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="B165">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C165">
         <v>4</v>
@@ -11015,27 +11016,32 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="B166">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C166">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>371</v>
+        <v>94</v>
       </c>
       <c r="B167">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C167">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{05AF3660-7BB6-4B35-A2B5-A126CAAF0875}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C167">
+      <sortCondition descending="1" ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
phutn update các view và control
</commit_message>
<xml_diff>
--- a/C500Hemis/TaiLieu/BangHemis.xlsx
+++ b/C500Hemis/TaiLieu/BangHemis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lap trinh may tinh\Code\C500Hemis\C500Hemis\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA35E70-7098-4D3F-A743-A1E8AD3A5517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF696B-CFCA-4C08-970D-0E6629EC0B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="98" yWindow="68" windowWidth="8399" windowHeight="12382" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tạo controller-B9" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DemTruong!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">LanAnh!$A$2:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Triển khai các controller'!$A$2:$C$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">View!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">View!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1586,6 +1586,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1594,12 +1600,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2025,10 +2025,10 @@
       <c r="B9" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="30">
         <v>8</v>
       </c>
     </row>
@@ -2039,8 +2039,8 @@
       <c r="B10" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="21">
@@ -2099,31 +2099,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="15" t="s">
         <v>293</v>
       </c>
@@ -11304,826 +11304,1115 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C87645-A414-4C17-8A6C-82C75FCFAF15}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.06640625" customWidth="1"/>
-    <col min="2" max="2" width="56.796875" customWidth="1"/>
-    <col min="3" max="3" width="28.796875" customWidth="1"/>
-    <col min="4" max="4" width="95.3984375" customWidth="1"/>
+    <col min="2" max="2" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.796875" customWidth="1"/>
+    <col min="4" max="4" width="28.796875" customWidth="1"/>
+    <col min="5" max="5" width="95.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>456</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="str">
+        <f>CONCATENATE(C2, "Controller")</f>
+        <v>vCoCauToChucController</v>
+      </c>
+      <c r="C2" t="s">
         <v>334</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">CONCATENATE(C3, "Controller")</f>
+        <v>vCoSoGiaoDucController</v>
+      </c>
+      <c r="C3" t="s">
         <v>370</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>vDanhHieuThiDuaGiaiThuongKhenThuongCuaCoSoGDController</v>
+      </c>
+      <c r="C4" t="s">
         <v>328</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>vDauMoiLienHeController</v>
+      </c>
+      <c r="C5" t="s">
         <v>308</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>vDonViLienKetDaoTaoGiaoDucController</v>
+      </c>
+      <c r="C6" t="s">
         <v>325</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>vKhoaHocController</v>
+      </c>
+      <c r="C7" t="s">
         <v>301</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>vLichSuDoiTenTruongController</v>
+      </c>
+      <c r="C8" t="s">
         <v>317</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>vToChucKiemDinhController</v>
+      </c>
+      <c r="C9" t="s">
         <v>321</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>vVanBanTuChuController</v>
+      </c>
+      <c r="C10" t="s">
         <v>320</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>vCongTrinhCoSoVatChatController</v>
+      </c>
+      <c r="C11" t="s">
         <v>357</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>vDatDaiController</v>
+      </c>
+      <c r="C12" t="s">
         <v>348</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>vKiTucXaController</v>
+      </c>
+      <c r="C13" t="s">
         <v>332</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>vPhongHocGiangDuongHoiTruongController</v>
+      </c>
+      <c r="C14" t="s">
         <v>353</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>vPhongThiNghiemController</v>
+      </c>
+      <c r="C15" t="s">
         <v>323</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>vPhongThucHanhController</v>
+      </c>
+      <c r="C16" t="s">
         <v>311</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>vThietBiPTN_THTren500TrController</v>
+      </c>
+      <c r="C17" t="s">
         <v>343</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>vThuVienTrungTamHocLieuController</v>
+      </c>
+      <c r="C18" t="s">
         <v>363</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>vChuongTrinhDaoTaoController</v>
+      </c>
+      <c r="C19" t="s">
         <v>366</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>76</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>vGiaHanChuongTrinhDaoTaoController</v>
+      </c>
+      <c r="C20" t="s">
         <v>326</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>76</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>vNamApdungChuongTrinhController</v>
+      </c>
+      <c r="C21" t="s">
         <v>329</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>76</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>vNgonNguGiangDayController</v>
+      </c>
+      <c r="C22" t="s">
         <v>313</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>vQuyetDinhCapPhepChuongTrinhDungChoChuongTrinhNuocNgoaiController</v>
+      </c>
+      <c r="C23" t="s">
         <v>330</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinKiemDinhCuaChuongTrinhController</v>
+      </c>
+      <c r="C24" t="s">
         <v>337</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>165</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>vNguoiController</v>
+      </c>
+      <c r="C25" t="s">
         <v>371</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>105</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>vToChucHopTacDoanhNghiepController</v>
+      </c>
+      <c r="C26" t="s">
         <v>338</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>109</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>vDeAnDuAnChuongTrinhController</v>
+      </c>
+      <c r="C27" t="s">
         <v>340</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>109</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>vDoanCongTacController</v>
+      </c>
+      <c r="C28" t="s">
         <v>352</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>109</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>vGVDuocCuDiDaoTaoController</v>
+      </c>
+      <c r="C29" t="s">
         <v>342</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>109</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>vHoiThaoHoiNghiController</v>
+      </c>
+      <c r="C30" t="s">
         <v>355</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>109</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>vLuuHocSinhSinhVienNNController</v>
+      </c>
+      <c r="C31" t="s">
         <v>304</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>109</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>vThanhPhanThamGiaDoanCongTacController</v>
+      </c>
+      <c r="C32" t="s">
         <v>306</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>109</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>vThoaThuanHopTacQuocTeController</v>
+      </c>
+      <c r="C33" t="s">
         <v>344</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>109</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinHopTacController</v>
+      </c>
+      <c r="C34" t="s">
         <v>351</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>109</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>vToChucHopTacQuocTeController</v>
+      </c>
+      <c r="C35" t="s">
         <v>339</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>137</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>vBaiBaoKHDaCongBoController</v>
+      </c>
+      <c r="C36" t="s">
         <v>356</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>137</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>vChuyenGiaoCongNgheVaDaoTaoController</v>
+      </c>
+      <c r="C37" t="s">
         <v>361</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>137</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>vDoanhNghiepKHCNController</v>
+      </c>
+      <c r="C38" t="s">
         <v>333</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>137</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>vDoiTuongThamGiaController</v>
+      </c>
+      <c r="C39" t="s">
         <v>324</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>137</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>vGiaiThuongKhoaHocController</v>
+      </c>
+      <c r="C40" t="s">
         <v>341</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>137</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>vHoatDongBaoVeMoiTruongController</v>
+      </c>
+      <c r="C41" t="s">
         <v>358</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>137</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>vNhiemVuKHCNController</v>
+      </c>
+      <c r="C42" t="s">
         <v>360</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>137</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>vNhomNghienCuuManhController</v>
+      </c>
+      <c r="C43" t="s">
         <v>331</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>137</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>vSachDaXuatBanController</v>
+      </c>
+      <c r="C44" t="s">
         <v>354</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>137</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>vTaiSanTriTueController</v>
+      </c>
+      <c r="C45" t="s">
         <v>362</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>137</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>vTapChiKhoaHocController</v>
+      </c>
+      <c r="C46" t="s">
         <v>335</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>175</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>vDanhSachNganhDaoTaoController</v>
+      </c>
+      <c r="C47" t="s">
         <v>367</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>175</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>vHinhThucDaoTaoCuaNganhController</v>
+      </c>
+      <c r="C48" t="s">
         <v>303</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>175</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>vKhoiNganhDaoTaoController</v>
+      </c>
+      <c r="C49" t="s">
         <v>300</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>175</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>vLoaiHinhDaoTaoKhacDuocChoPhepMoNganhController</v>
+      </c>
+      <c r="C50" t="s">
         <v>318</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>175</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>vNhomNganhDaoTaoController</v>
+      </c>
+      <c r="C51" t="s">
         <v>305</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>175</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinLinhVucDaoTaoController</v>
+      </c>
+      <c r="C52" t="s">
         <v>302</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>200</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>vDanhHieuThiDuaGiaiThuongKhenThuongNguoiHocController</v>
+      </c>
+      <c r="C53" t="s">
         <v>349</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>200</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>vHocVienController</v>
+      </c>
+      <c r="C54" t="s">
         <v>364</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>200</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>vKyLuatNguoiHocController</v>
+      </c>
+      <c r="C55" t="s">
         <v>347</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>200</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>vNguoiHocVayTinDungController</v>
+      </c>
+      <c r="C56" t="s">
         <v>346</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>200</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinHocBongController</v>
+      </c>
+      <c r="C57" t="s">
         <v>345</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>200</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinHocTapNghienCuuSinhController</v>
+      </c>
+      <c r="C58" t="s">
         <v>369</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>200</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinHocTapSinhVienController</v>
+      </c>
+      <c r="C59" t="s">
         <v>368</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>200</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinNguoiHocGDTCController</v>
+      </c>
+      <c r="C60" t="s">
         <v>322</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>200</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinViecLamSauTotNghiepController</v>
+      </c>
+      <c r="C61" t="s">
         <v>350</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>200</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>vThongTinViPhamController</v>
+      </c>
+      <c r="C62" t="s">
         <v>336</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>411</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>database_firewall_rulesController</v>
+      </c>
+      <c r="C63" t="s">
         <v>412</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>1</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>vChiTietTaiSanDonViController</v>
+      </c>
+      <c r="C64" t="s">
         <v>327</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>1</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>vChiTietThuChiController</v>
+      </c>
+      <c r="C65" t="s">
         <v>309</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>1</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>vHoatDongTaiChinhController</v>
+      </c>
+      <c r="C66" t="s">
         <v>314</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>1</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B73" si="1">CONCATENATE(C67, "Controller")</f>
+        <v>vKhoanNopNganSachController</v>
+      </c>
+      <c r="C67" t="s">
         <v>315</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>1</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>vKhoanTrichLapQuyController</v>
+      </c>
+      <c r="C68" t="s">
         <v>316</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>1</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>vLoaiThuChiController</v>
+      </c>
+      <c r="C69" t="s">
         <v>319</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>1</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>vTaiSanDonViController</v>
+      </c>
+      <c r="C70" t="s">
         <v>312</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>25</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>vChiTieuTuyenSinhTheoNganhController</v>
+      </c>
+      <c r="C71" t="s">
         <v>310</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>25</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>vDuLieuTrungTuyenController</v>
+      </c>
+      <c r="C72" t="s">
         <v>365</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>34</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>vDanhSachVanBangChungChiController</v>
+      </c>
+      <c r="C73" t="s">
         <v>359</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>454</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{A0C87645-A414-4C17-8A6C-82C75FCFAF15}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F73">
+  <autoFilter ref="A1:G1" xr:uid="{A0C87645-A414-4C17-8A6C-82C75FCFAF15}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G73">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
@@ -16195,7 +16484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4A2D16-A3A0-47BE-B691-95D6AE66D8F8}">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B93" sqref="B93:B95"/>
     </sheetView>
   </sheetViews>
@@ -16210,33 +16499,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="7"/>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="31" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="28"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="str">
+      <c r="B3" s="27" t="str">
         <f>CONCATENATE(C3,"Controller")</f>
         <v>QuaTrinhCongTacCuaCanBoController</v>
       </c>
-      <c r="C3" s="30" t="str">
+      <c r="C3" s="27" t="str">
         <f>RIGHT(D3,LEN(D3)-2)</f>
         <v>QuaTrinhCongTacCuaCanBo</v>
       </c>
@@ -16251,11 +16540,11 @@
       <c r="A4" s="17">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="str">
+      <c r="B4" s="27" t="str">
         <f t="shared" ref="B4:B67" si="0">CONCATENATE(C4,"Controller")</f>
         <v>QuaTrinhDaoTaoCuaCanBoController</v>
       </c>
-      <c r="C4" s="30" t="str">
+      <c r="C4" s="27" t="str">
         <f t="shared" ref="C4:C67" si="1">RIGHT(D4,LEN(D4)-2)</f>
         <v>QuaTrinhDaoTaoCuaCanBo</v>
       </c>
@@ -16270,11 +16559,11 @@
       <c r="A5" s="17">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="str">
+      <c r="B5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>TrinhDoTiengDanTocController</v>
       </c>
-      <c r="C5" s="30" t="str">
+      <c r="C5" s="27" t="str">
         <f t="shared" si="1"/>
         <v>TrinhDoTiengDanToc</v>
       </c>
@@ -16289,11 +16578,11 @@
       <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="str">
+      <c r="B6" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CanBoController</v>
       </c>
-      <c r="C6" s="30" t="str">
+      <c r="C6" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CanBo</v>
       </c>
@@ -16308,11 +16597,11 @@
       <c r="A7" s="17">
         <v>5</v>
       </c>
-      <c r="B7" s="30" t="str">
+      <c r="B7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CanBoHuongDanThanhCongSinhVienController</v>
       </c>
-      <c r="C7" s="30" t="str">
+      <c r="C7" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CanBoHuongDanThanhCongSinhVien</v>
       </c>
@@ -16327,11 +16616,11 @@
       <c r="A8" s="17">
         <v>6</v>
       </c>
-      <c r="B8" s="30" t="str">
+      <c r="B8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ChucDanhKhoaHocCuaCanBoController</v>
       </c>
-      <c r="C8" s="30" t="str">
+      <c r="C8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ChucDanhKhoaHocCuaCanBo</v>
       </c>
@@ -16346,11 +16635,11 @@
       <c r="A9" s="17">
         <v>7</v>
       </c>
-      <c r="B9" s="30" t="str">
+      <c r="B9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DanhGiaXepLoaiCanBoController</v>
       </c>
-      <c r="C9" s="30" t="str">
+      <c r="C9" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DanhGiaXepLoaiCanBo</v>
       </c>
@@ -16365,11 +16654,11 @@
       <c r="A10" s="17">
         <v>8</v>
       </c>
-      <c r="B10" s="30" t="str">
+      <c r="B10" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongCanBoController</v>
       </c>
-      <c r="C10" s="30" t="str">
+      <c r="C10" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongCanBo</v>
       </c>
@@ -16384,11 +16673,11 @@
       <c r="A11" s="17">
         <v>9</v>
       </c>
-      <c r="B11" s="30" t="str">
+      <c r="B11" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DienBienLuongController</v>
       </c>
-      <c r="C11" s="30" t="str">
+      <c r="C11" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DienBienLuong</v>
       </c>
@@ -16403,11 +16692,11 @@
       <c r="A12" s="17">
         <v>10</v>
       </c>
-      <c r="B12" s="30" t="str">
+      <c r="B12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DoiTuongChinhSachCanBoController</v>
       </c>
-      <c r="C12" s="30" t="str">
+      <c r="C12" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DoiTuongChinhSachCanBo</v>
       </c>
@@ -16422,11 +16711,11 @@
       <c r="A13" s="17">
         <v>11</v>
       </c>
-      <c r="B13" s="30" t="str">
+      <c r="B13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DonViCongTacCuaCanBoController</v>
       </c>
-      <c r="C13" s="30" t="str">
+      <c r="C13" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DonViCongTacCuaCanBo</v>
       </c>
@@ -16441,11 +16730,11 @@
       <c r="A14" s="17">
         <v>12</v>
       </c>
-      <c r="B14" s="30" t="str">
+      <c r="B14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DonViThinhGiangCuaCanBoController</v>
       </c>
-      <c r="C14" s="30" t="str">
+      <c r="C14" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DonViThinhGiangCuaCanBo</v>
       </c>
@@ -16460,11 +16749,11 @@
       <c r="A15" s="11">
         <v>13</v>
       </c>
-      <c r="B15" s="30" t="str">
+      <c r="B15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GiangVienNNController</v>
       </c>
-      <c r="C15" s="30" t="str">
+      <c r="C15" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GiangVienNN</v>
       </c>
@@ -16479,11 +16768,11 @@
       <c r="A16" s="11">
         <v>14</v>
       </c>
-      <c r="B16" s="30" t="str">
+      <c r="B16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GiaoVienQPANController</v>
       </c>
-      <c r="C16" s="30" t="str">
+      <c r="C16" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GiaoVienQPAN</v>
       </c>
@@ -16498,11 +16787,11 @@
       <c r="A17" s="11">
         <v>15</v>
       </c>
-      <c r="B17" s="30" t="str">
+      <c r="B17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>HopDongController</v>
       </c>
-      <c r="C17" s="30" t="str">
+      <c r="C17" s="27" t="str">
         <f t="shared" si="1"/>
         <v>HopDong</v>
       </c>
@@ -16517,11 +16806,11 @@
       <c r="A18" s="11">
         <v>16</v>
       </c>
-      <c r="B18" s="30" t="str">
+      <c r="B18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>HopDongThinhGiangController</v>
       </c>
-      <c r="C18" s="30" t="str">
+      <c r="C18" s="27" t="str">
         <f t="shared" si="1"/>
         <v>HopDongThinhGiang</v>
       </c>
@@ -16536,11 +16825,11 @@
       <c r="A19" s="11">
         <v>17</v>
       </c>
-      <c r="B19" s="30" t="str">
+      <c r="B19" s="27" t="str">
         <f t="shared" si="0"/>
         <v>KhoaBoiDuongTapHuanThamGiaCuaCanBoController</v>
       </c>
-      <c r="C19" s="30" t="str">
+      <c r="C19" s="27" t="str">
         <f t="shared" si="1"/>
         <v>KhoaBoiDuongTapHuanThamGiaCuaCanBo</v>
       </c>
@@ -16555,11 +16844,11 @@
       <c r="A20" s="11">
         <v>18</v>
       </c>
-      <c r="B20" s="30" t="str">
+      <c r="B20" s="27" t="str">
         <f t="shared" si="0"/>
         <v>KyLuatCanBoController</v>
       </c>
-      <c r="C20" s="30" t="str">
+      <c r="C20" s="27" t="str">
         <f t="shared" si="1"/>
         <v>KyLuatCanBo</v>
       </c>
@@ -16574,11 +16863,11 @@
       <c r="A21" s="11">
         <v>19</v>
       </c>
-      <c r="B21" s="30" t="str">
+      <c r="B21" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LinhVucNghienCuuCuaCanBoController</v>
       </c>
-      <c r="C21" s="30" t="str">
+      <c r="C21" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LinhVucNghienCuuCuaCanBo</v>
       </c>
@@ -16593,11 +16882,11 @@
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="30" t="str">
+      <c r="B22" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NganhDungTenGiangDayController</v>
       </c>
-      <c r="C22" s="30" t="str">
+      <c r="C22" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NganhDungTenGiangDay</v>
       </c>
@@ -16612,11 +16901,11 @@
       <c r="A23" s="11">
         <v>21</v>
       </c>
-      <c r="B23" s="30" t="str">
+      <c r="B23" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NganhGiangDayCuaCanBoController</v>
       </c>
-      <c r="C23" s="30" t="str">
+      <c r="C23" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NganhGiangDayCuaCanBo</v>
       </c>
@@ -16631,11 +16920,11 @@
       <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" s="30" t="str">
+      <c r="B24" s="27" t="str">
         <f t="shared" si="0"/>
         <v>PhuCapController</v>
       </c>
-      <c r="C24" s="30" t="str">
+      <c r="C24" s="27" t="str">
         <f t="shared" si="1"/>
         <v>PhuCap</v>
       </c>
@@ -16650,11 +16939,11 @@
       <c r="A25" s="13">
         <v>23</v>
       </c>
-      <c r="B25" s="30" t="str">
+      <c r="B25" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CoCauToChucController</v>
       </c>
-      <c r="C25" s="30" t="str">
+      <c r="C25" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CoCauToChuc</v>
       </c>
@@ -16669,11 +16958,11 @@
       <c r="A26" s="13">
         <v>24</v>
       </c>
-      <c r="B26" s="30" t="str">
+      <c r="B26" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CoSoGiaoDucController</v>
       </c>
-      <c r="C26" s="30" t="str">
+      <c r="C26" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CoSoGiaoDuc</v>
       </c>
@@ -16688,11 +16977,11 @@
       <c r="A27" s="9">
         <v>25</v>
       </c>
-      <c r="B27" s="30" t="str">
+      <c r="B27" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongCuaCoSoGDController</v>
       </c>
-      <c r="C27" s="30" t="str">
+      <c r="C27" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongCuaCoSoGD</v>
       </c>
@@ -16707,11 +16996,11 @@
       <c r="A28" s="9">
         <v>26</v>
       </c>
-      <c r="B28" s="30" t="str">
+      <c r="B28" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DauMoiLienHeController</v>
       </c>
-      <c r="C28" s="30" t="str">
+      <c r="C28" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DauMoiLienHe</v>
       </c>
@@ -16726,11 +17015,11 @@
       <c r="A29" s="9">
         <v>27</v>
       </c>
-      <c r="B29" s="30" t="str">
+      <c r="B29" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DonViLienKetDaoTaoGiaoDucController</v>
       </c>
-      <c r="C29" s="30" t="str">
+      <c r="C29" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DonViLienKetDaoTaoGiaoDuc</v>
       </c>
@@ -16745,11 +17034,11 @@
       <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="30" t="str">
+      <c r="B30" s="27" t="str">
         <f t="shared" si="0"/>
         <v>KhoaHocController</v>
       </c>
-      <c r="C30" s="30" t="str">
+      <c r="C30" s="27" t="str">
         <f t="shared" si="1"/>
         <v>KhoaHoc</v>
       </c>
@@ -16764,11 +17053,11 @@
       <c r="A31" s="9">
         <v>29</v>
       </c>
-      <c r="B31" s="30" t="str">
+      <c r="B31" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LichSuDoiTenTruongController</v>
       </c>
-      <c r="C31" s="30" t="str">
+      <c r="C31" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LichSuDoiTenTruong</v>
       </c>
@@ -16783,11 +17072,11 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="30" t="str">
+      <c r="B32" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ToChucKiemDinhController</v>
       </c>
-      <c r="C32" s="30" t="str">
+      <c r="C32" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ToChucKiemDinh</v>
       </c>
@@ -16802,11 +17091,11 @@
       <c r="A33" s="9">
         <v>31</v>
       </c>
-      <c r="B33" s="30" t="str">
+      <c r="B33" s="27" t="str">
         <f t="shared" si="0"/>
         <v>VanBanTuChuController</v>
       </c>
-      <c r="C33" s="30" t="str">
+      <c r="C33" s="27" t="str">
         <f t="shared" si="1"/>
         <v>VanBanTuChu</v>
       </c>
@@ -16821,11 +17110,11 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="30" t="str">
+      <c r="B34" s="27" t="str">
         <f t="shared" si="0"/>
         <v>CongTrinhCoSoVatChatController</v>
       </c>
-      <c r="C34" s="30" t="str">
+      <c r="C34" s="27" t="str">
         <f t="shared" si="1"/>
         <v>CongTrinhCoSoVatChat</v>
       </c>
@@ -16840,11 +17129,11 @@
       <c r="A35" s="9">
         <v>33</v>
       </c>
-      <c r="B35" s="30" t="str">
+      <c r="B35" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DatDaiController</v>
       </c>
-      <c r="C35" s="30" t="str">
+      <c r="C35" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DatDai</v>
       </c>
@@ -16859,11 +17148,11 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="30" t="str">
+      <c r="B36" s="27" t="str">
         <f t="shared" si="0"/>
         <v>KiTucXaController</v>
       </c>
-      <c r="C36" s="30" t="str">
+      <c r="C36" s="27" t="str">
         <f t="shared" si="1"/>
         <v>KiTucXa</v>
       </c>
@@ -16878,11 +17167,11 @@
       <c r="A37" s="9">
         <v>35</v>
       </c>
-      <c r="B37" s="30" t="str">
+      <c r="B37" s="27" t="str">
         <f t="shared" si="0"/>
         <v>PhongHocGiangDuongHoiTruongController</v>
       </c>
-      <c r="C37" s="30" t="str">
+      <c r="C37" s="27" t="str">
         <f t="shared" si="1"/>
         <v>PhongHocGiangDuongHoiTruong</v>
       </c>
@@ -16897,11 +17186,11 @@
       <c r="A38" s="9">
         <v>36</v>
       </c>
-      <c r="B38" s="30" t="str">
+      <c r="B38" s="27" t="str">
         <f t="shared" si="0"/>
         <v>PhongThiNghiemController</v>
       </c>
-      <c r="C38" s="30" t="str">
+      <c r="C38" s="27" t="str">
         <f t="shared" si="1"/>
         <v>PhongThiNghiem</v>
       </c>
@@ -16916,11 +17205,11 @@
       <c r="A39" s="9">
         <v>37</v>
       </c>
-      <c r="B39" s="30" t="str">
+      <c r="B39" s="27" t="str">
         <f t="shared" si="0"/>
         <v>PhongThucHanhController</v>
       </c>
-      <c r="C39" s="30" t="str">
+      <c r="C39" s="27" t="str">
         <f t="shared" si="1"/>
         <v>PhongThucHanh</v>
       </c>
@@ -16935,11 +17224,11 @@
       <c r="A40" s="9">
         <v>38</v>
       </c>
-      <c r="B40" s="30" t="str">
+      <c r="B40" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThietBiPTN_THTren500TrController</v>
       </c>
-      <c r="C40" s="30" t="str">
+      <c r="C40" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThietBiPTN_THTren500Tr</v>
       </c>
@@ -16954,11 +17243,11 @@
       <c r="A41" s="9">
         <v>39</v>
       </c>
-      <c r="B41" s="30" t="str">
+      <c r="B41" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThuVienTrungTamHocLieuController</v>
       </c>
-      <c r="C41" s="30" t="str">
+      <c r="C41" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThuVienTrungTamHocLieu</v>
       </c>
@@ -16973,11 +17262,11 @@
       <c r="A42" s="9">
         <v>40</v>
       </c>
-      <c r="B42" s="30" t="str">
+      <c r="B42" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ChuongTrinhDaoTaoController</v>
       </c>
-      <c r="C42" s="30" t="str">
+      <c r="C42" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ChuongTrinhDaoTao</v>
       </c>
@@ -16992,11 +17281,11 @@
       <c r="A43" s="9">
         <v>41</v>
       </c>
-      <c r="B43" s="30" t="str">
+      <c r="B43" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GiaHanChuongTrinhDaoTaoController</v>
       </c>
-      <c r="C43" s="30" t="str">
+      <c r="C43" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GiaHanChuongTrinhDaoTao</v>
       </c>
@@ -17011,11 +17300,11 @@
       <c r="A44" s="9">
         <v>42</v>
       </c>
-      <c r="B44" s="30" t="str">
+      <c r="B44" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NamApDungChuongTrinhController</v>
       </c>
-      <c r="C44" s="30" t="str">
+      <c r="C44" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NamApDungChuongTrinh</v>
       </c>
@@ -17030,11 +17319,11 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="30" t="str">
+      <c r="B45" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NgonNguGiangDayController</v>
       </c>
-      <c r="C45" s="30" t="str">
+      <c r="C45" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NgonNguGiangDay</v>
       </c>
@@ -17049,11 +17338,11 @@
       <c r="A46" s="9">
         <v>44</v>
       </c>
-      <c r="B46" s="30" t="str">
+      <c r="B46" s="27" t="str">
         <f t="shared" si="0"/>
         <v>QuyetDinhCapPhepChuongTrinhDungChoChuongTrinhNuocNgoaiController</v>
       </c>
-      <c r="C46" s="30" t="str">
+      <c r="C46" s="27" t="str">
         <f t="shared" si="1"/>
         <v>QuyetDinhCapPhepChuongTrinhDungChoChuongTrinhNuocNgoai</v>
       </c>
@@ -17068,11 +17357,11 @@
       <c r="A47" s="9">
         <v>45</v>
       </c>
-      <c r="B47" s="30" t="str">
+      <c r="B47" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThongTinKiemDinhCuaChuongTrinhController</v>
       </c>
-      <c r="C47" s="30" t="str">
+      <c r="C47" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThongTinKiemDinhCuaChuongTrinh</v>
       </c>
@@ -17087,11 +17376,11 @@
       <c r="A48" s="9">
         <v>46</v>
       </c>
-      <c r="B48" s="30" t="str">
+      <c r="B48" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NguoiController</v>
       </c>
-      <c r="C48" s="30" t="str">
+      <c r="C48" s="27" t="str">
         <f t="shared" si="1"/>
         <v>Nguoi</v>
       </c>
@@ -17106,11 +17395,11 @@
       <c r="A49" s="9">
         <v>47</v>
       </c>
-      <c r="B49" s="30" t="str">
+      <c r="B49" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ToChucHopTacDoanhNghiepController</v>
       </c>
-      <c r="C49" s="30" t="str">
+      <c r="C49" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ToChucHopTacDoanhNghiep</v>
       </c>
@@ -17125,11 +17414,11 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="30" t="str">
+      <c r="B50" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DeAnDuAnChuongTrinhController</v>
       </c>
-      <c r="C50" s="30" t="str">
+      <c r="C50" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DeAnDuAnChuongTrinh</v>
       </c>
@@ -17144,11 +17433,11 @@
       <c r="A51" s="9">
         <v>49</v>
       </c>
-      <c r="B51" s="30" t="str">
+      <c r="B51" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DoanCongTacController</v>
       </c>
-      <c r="C51" s="30" t="str">
+      <c r="C51" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DoanCongTac</v>
       </c>
@@ -17163,11 +17452,11 @@
       <c r="A52" s="9">
         <v>50</v>
       </c>
-      <c r="B52" s="30" t="str">
+      <c r="B52" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GVDuocCuDiDaoTaoController</v>
       </c>
-      <c r="C52" s="30" t="str">
+      <c r="C52" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GVDuocCuDiDaoTao</v>
       </c>
@@ -17182,11 +17471,11 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="30" t="str">
+      <c r="B53" s="27" t="str">
         <f t="shared" si="0"/>
         <v>HoiThaoHoiNghiController</v>
       </c>
-      <c r="C53" s="30" t="str">
+      <c r="C53" s="27" t="str">
         <f t="shared" si="1"/>
         <v>HoiThaoHoiNghi</v>
       </c>
@@ -17201,11 +17490,11 @@
       <c r="A54" s="9">
         <v>52</v>
       </c>
-      <c r="B54" s="30" t="str">
+      <c r="B54" s="27" t="str">
         <f t="shared" si="0"/>
         <v>LuuHocSinhSinhVienNNController</v>
       </c>
-      <c r="C54" s="30" t="str">
+      <c r="C54" s="27" t="str">
         <f t="shared" si="1"/>
         <v>LuuHocSinhSinhVienNN</v>
       </c>
@@ -17220,11 +17509,11 @@
       <c r="A55" s="9">
         <v>53</v>
       </c>
-      <c r="B55" s="30" t="str">
+      <c r="B55" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThanhPhanThamGiaDoanCongTacController</v>
       </c>
-      <c r="C55" s="30" t="str">
+      <c r="C55" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThanhPhanThamGiaDoanCongTac</v>
       </c>
@@ -17239,11 +17528,11 @@
       <c r="A56" s="9">
         <v>54</v>
       </c>
-      <c r="B56" s="30" t="str">
+      <c r="B56" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThoaThuanHopTacQuocTeController</v>
       </c>
-      <c r="C56" s="30" t="str">
+      <c r="C56" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThoaThuanHopTacQuocTe</v>
       </c>
@@ -17258,11 +17547,11 @@
       <c r="A57" s="9">
         <v>55</v>
       </c>
-      <c r="B57" s="30" t="str">
+      <c r="B57" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ThongTinHopTacController</v>
       </c>
-      <c r="C57" s="30" t="str">
+      <c r="C57" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ThongTinHopTac</v>
       </c>
@@ -17277,11 +17566,11 @@
       <c r="A58" s="9">
         <v>56</v>
       </c>
-      <c r="B58" s="30" t="str">
+      <c r="B58" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ToChucHopTacQuocTeController</v>
       </c>
-      <c r="C58" s="30" t="str">
+      <c r="C58" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ToChucHopTacQuocTe</v>
       </c>
@@ -17296,11 +17585,11 @@
       <c r="A59" s="9">
         <v>57</v>
       </c>
-      <c r="B59" s="30" t="str">
+      <c r="B59" s="27" t="str">
         <f t="shared" si="0"/>
         <v>BaiBaoKHDaCongBoController</v>
       </c>
-      <c r="C59" s="30" t="str">
+      <c r="C59" s="27" t="str">
         <f t="shared" si="1"/>
         <v>BaiBaoKHDaCongBo</v>
       </c>
@@ -17315,11 +17604,11 @@
       <c r="A60" s="9">
         <v>58</v>
       </c>
-      <c r="B60" s="30" t="str">
+      <c r="B60" s="27" t="str">
         <f t="shared" si="0"/>
         <v>ChuyenGiaoCongNgheVaDaoTaoController</v>
       </c>
-      <c r="C60" s="30" t="str">
+      <c r="C60" s="27" t="str">
         <f t="shared" si="1"/>
         <v>ChuyenGiaoCongNgheVaDaoTao</v>
       </c>
@@ -17334,11 +17623,11 @@
       <c r="A61" s="9">
         <v>59</v>
       </c>
-      <c r="B61" s="30" t="str">
+      <c r="B61" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DoanhNghiepKHCNController</v>
       </c>
-      <c r="C61" s="30" t="str">
+      <c r="C61" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DoanhNghiepKHCN</v>
       </c>
@@ -17353,11 +17642,11 @@
       <c r="A62" s="9">
         <v>60</v>
       </c>
-      <c r="B62" s="30" t="str">
+      <c r="B62" s="27" t="str">
         <f t="shared" si="0"/>
         <v>DoiTuongThamGiaController</v>
       </c>
-      <c r="C62" s="30" t="str">
+      <c r="C62" s="27" t="str">
         <f t="shared" si="1"/>
         <v>DoiTuongThamGia</v>
       </c>
@@ -17372,11 +17661,11 @@
       <c r="A63" s="9">
         <v>61</v>
       </c>
-      <c r="B63" s="30" t="str">
+      <c r="B63" s="27" t="str">
         <f t="shared" si="0"/>
         <v>GiaiThuongKhoaHocController</v>
       </c>
-      <c r="C63" s="30" t="str">
+      <c r="C63" s="27" t="str">
         <f t="shared" si="1"/>
         <v>GiaiThuongKhoaHoc</v>
       </c>
@@ -17391,11 +17680,11 @@
       <c r="A64" s="9">
         <v>62</v>
       </c>
-      <c r="B64" s="30" t="str">
+      <c r="B64" s="27" t="str">
         <f t="shared" si="0"/>
         <v>HoatDongBaoVeMoiTruongController</v>
       </c>
-      <c r="C64" s="30" t="str">
+      <c r="C64" s="27" t="str">
         <f t="shared" si="1"/>
         <v>HoatDongBaoVeMoiTruong</v>
       </c>
@@ -17410,11 +17699,11 @@
       <c r="A65" s="9">
         <v>63</v>
       </c>
-      <c r="B65" s="30" t="str">
+      <c r="B65" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NhiemVuKHCNController</v>
       </c>
-      <c r="C65" s="30" t="str">
+      <c r="C65" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NhiemVuKHCN</v>
       </c>
@@ -17429,11 +17718,11 @@
       <c r="A66" s="9">
         <v>64</v>
       </c>
-      <c r="B66" s="30" t="str">
+      <c r="B66" s="27" t="str">
         <f t="shared" si="0"/>
         <v>NhomNghienCuuManhController</v>
       </c>
-      <c r="C66" s="30" t="str">
+      <c r="C66" s="27" t="str">
         <f t="shared" si="1"/>
         <v>NhomNghienCuuManh</v>
       </c>
@@ -17448,11 +17737,11 @@
       <c r="A67" s="9">
         <v>65</v>
       </c>
-      <c r="B67" s="30" t="str">
+      <c r="B67" s="27" t="str">
         <f t="shared" si="0"/>
         <v>SachDaXuatBanController</v>
       </c>
-      <c r="C67" s="30" t="str">
+      <c r="C67" s="27" t="str">
         <f t="shared" si="1"/>
         <v>SachDaXuatBan</v>
       </c>
@@ -17467,11 +17756,11 @@
       <c r="A68" s="9">
         <v>66</v>
       </c>
-      <c r="B68" s="30" t="str">
+      <c r="B68" s="27" t="str">
         <f t="shared" ref="B68:B95" si="2">CONCATENATE(C68,"Controller")</f>
         <v>TaiSanTriTueController</v>
       </c>
-      <c r="C68" s="30" t="str">
+      <c r="C68" s="27" t="str">
         <f t="shared" ref="C68:C95" si="3">RIGHT(D68,LEN(D68)-2)</f>
         <v>TaiSanTriTue</v>
       </c>
@@ -17486,11 +17775,11 @@
       <c r="A69" s="9">
         <v>67</v>
       </c>
-      <c r="B69" s="30" t="str">
+      <c r="B69" s="27" t="str">
         <f t="shared" si="2"/>
         <v>TapChiKhoaHocController</v>
       </c>
-      <c r="C69" s="30" t="str">
+      <c r="C69" s="27" t="str">
         <f t="shared" si="3"/>
         <v>TapChiKhoaHoc</v>
       </c>
@@ -17505,11 +17794,11 @@
       <c r="A70" s="9">
         <v>68</v>
       </c>
-      <c r="B70" s="30" t="str">
+      <c r="B70" s="27" t="str">
         <f t="shared" si="2"/>
         <v>DanhSachNganhDaoTaoController</v>
       </c>
-      <c r="C70" s="30" t="str">
+      <c r="C70" s="27" t="str">
         <f t="shared" si="3"/>
         <v>DanhSachNganhDaoTao</v>
       </c>
@@ -17524,11 +17813,11 @@
       <c r="A71" s="9">
         <v>69</v>
       </c>
-      <c r="B71" s="30" t="str">
+      <c r="B71" s="27" t="str">
         <f t="shared" si="2"/>
         <v>HinhThucDaoTaoCuaNganhController</v>
       </c>
-      <c r="C71" s="30" t="str">
+      <c r="C71" s="27" t="str">
         <f t="shared" si="3"/>
         <v>HinhThucDaoTaoCuaNganh</v>
       </c>
@@ -17543,11 +17832,11 @@
       <c r="A72" s="9">
         <v>70</v>
       </c>
-      <c r="B72" s="30" t="str">
+      <c r="B72" s="27" t="str">
         <f t="shared" si="2"/>
         <v>KhoiNganhDaoTaoController</v>
       </c>
-      <c r="C72" s="30" t="str">
+      <c r="C72" s="27" t="str">
         <f t="shared" si="3"/>
         <v>KhoiNganhDaoTao</v>
       </c>
@@ -17562,11 +17851,11 @@
       <c r="A73" s="9">
         <v>71</v>
       </c>
-      <c r="B73" s="30" t="str">
+      <c r="B73" s="27" t="str">
         <f t="shared" si="2"/>
         <v>LoaiHinhDaoTaoKhacDuocChoPhepMoNganhController</v>
       </c>
-      <c r="C73" s="30" t="str">
+      <c r="C73" s="27" t="str">
         <f t="shared" si="3"/>
         <v>LoaiHinhDaoTaoKhacDuocChoPhepMoNganh</v>
       </c>
@@ -17581,11 +17870,11 @@
       <c r="A74" s="9">
         <v>72</v>
       </c>
-      <c r="B74" s="30" t="str">
+      <c r="B74" s="27" t="str">
         <f t="shared" si="2"/>
         <v>NhomNganhDaoTaoController</v>
       </c>
-      <c r="C74" s="30" t="str">
+      <c r="C74" s="27" t="str">
         <f t="shared" si="3"/>
         <v>NhomNganhDaoTao</v>
       </c>
@@ -17600,11 +17889,11 @@
       <c r="A75" s="9">
         <v>73</v>
       </c>
-      <c r="B75" s="30" t="str">
+      <c r="B75" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinLinhVucDaoTaoController</v>
       </c>
-      <c r="C75" s="30" t="str">
+      <c r="C75" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinLinhVucDaoTao</v>
       </c>
@@ -17619,11 +17908,11 @@
       <c r="A76" s="9">
         <v>74</v>
       </c>
-      <c r="B76" s="30" t="str">
+      <c r="B76" s="27" t="str">
         <f t="shared" si="2"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongNguoiHocController</v>
       </c>
-      <c r="C76" s="30" t="str">
+      <c r="C76" s="27" t="str">
         <f t="shared" si="3"/>
         <v>DanhHieuThiDuaGiaiThuongKhenThuongNguoiHoc</v>
       </c>
@@ -17638,11 +17927,11 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="30" t="str">
+      <c r="B77" s="27" t="str">
         <f t="shared" si="2"/>
         <v>HocVienController</v>
       </c>
-      <c r="C77" s="30" t="str">
+      <c r="C77" s="27" t="str">
         <f t="shared" si="3"/>
         <v>HocVien</v>
       </c>
@@ -17657,11 +17946,11 @@
       <c r="A78" s="9">
         <v>76</v>
       </c>
-      <c r="B78" s="30" t="str">
+      <c r="B78" s="27" t="str">
         <f t="shared" si="2"/>
         <v>KyLuatNguoiHocController</v>
       </c>
-      <c r="C78" s="30" t="str">
+      <c r="C78" s="27" t="str">
         <f t="shared" si="3"/>
         <v>KyLuatNguoiHoc</v>
       </c>
@@ -17676,11 +17965,11 @@
       <c r="A79" s="9">
         <v>77</v>
       </c>
-      <c r="B79" s="30" t="str">
+      <c r="B79" s="27" t="str">
         <f t="shared" si="2"/>
         <v>NguoiHocVayTinDungController</v>
       </c>
-      <c r="C79" s="30" t="str">
+      <c r="C79" s="27" t="str">
         <f t="shared" si="3"/>
         <v>NguoiHocVayTinDung</v>
       </c>
@@ -17695,11 +17984,11 @@
       <c r="A80" s="9">
         <v>78</v>
       </c>
-      <c r="B80" s="30" t="str">
+      <c r="B80" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinHocBongController</v>
       </c>
-      <c r="C80" s="30" t="str">
+      <c r="C80" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinHocBong</v>
       </c>
@@ -17714,11 +18003,11 @@
       <c r="A81" s="9">
         <v>79</v>
       </c>
-      <c r="B81" s="30" t="str">
+      <c r="B81" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinHocTapNghienCuuSinhController</v>
       </c>
-      <c r="C81" s="30" t="str">
+      <c r="C81" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinHocTapNghienCuuSinh</v>
       </c>
@@ -17733,11 +18022,11 @@
       <c r="A82" s="9">
         <v>80</v>
       </c>
-      <c r="B82" s="30" t="str">
+      <c r="B82" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinHocTapSinhVienController</v>
       </c>
-      <c r="C82" s="30" t="str">
+      <c r="C82" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinHocTapSinhVien</v>
       </c>
@@ -17752,11 +18041,11 @@
       <c r="A83" s="9">
         <v>81</v>
       </c>
-      <c r="B83" s="30" t="str">
+      <c r="B83" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinNguoiHocGDTCController</v>
       </c>
-      <c r="C83" s="30" t="str">
+      <c r="C83" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinNguoiHocGDTC</v>
       </c>
@@ -17771,11 +18060,11 @@
       <c r="A84" s="9">
         <v>82</v>
       </c>
-      <c r="B84" s="30" t="str">
+      <c r="B84" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinViecLamSauTotNghiepController</v>
       </c>
-      <c r="C84" s="30" t="str">
+      <c r="C84" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinViecLamSauTotNghiep</v>
       </c>
@@ -17790,11 +18079,11 @@
       <c r="A85" s="9">
         <v>83</v>
       </c>
-      <c r="B85" s="30" t="str">
+      <c r="B85" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ThongTinViPhamController</v>
       </c>
-      <c r="C85" s="30" t="str">
+      <c r="C85" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ThongTinViPham</v>
       </c>
@@ -17809,11 +18098,11 @@
       <c r="A86" s="9">
         <v>84</v>
       </c>
-      <c r="B86" s="30" t="str">
+      <c r="B86" s="27" t="str">
         <f t="shared" si="2"/>
         <v>HoatDongTaiChinhController</v>
       </c>
-      <c r="C86" s="30" t="str">
+      <c r="C86" s="27" t="str">
         <f t="shared" si="3"/>
         <v>HoatDongTaiChinh</v>
       </c>
@@ -17828,11 +18117,11 @@
       <c r="A87" s="9">
         <v>85</v>
       </c>
-      <c r="B87" s="30" t="str">
+      <c r="B87" s="27" t="str">
         <f t="shared" si="2"/>
         <v>KhoanNopNganSachController</v>
       </c>
-      <c r="C87" s="30" t="str">
+      <c r="C87" s="27" t="str">
         <f t="shared" si="3"/>
         <v>KhoanNopNganSach</v>
       </c>
@@ -17847,11 +18136,11 @@
       <c r="A88" s="9">
         <v>86</v>
       </c>
-      <c r="B88" s="30" t="str">
+      <c r="B88" s="27" t="str">
         <f t="shared" si="2"/>
         <v>KhoanTrichLapQuyController</v>
       </c>
-      <c r="C88" s="30" t="str">
+      <c r="C88" s="27" t="str">
         <f t="shared" si="3"/>
         <v>KhoanTrichLapQuy</v>
       </c>
@@ -17866,11 +18155,11 @@
       <c r="A89" s="9">
         <v>87</v>
       </c>
-      <c r="B89" s="30" t="str">
+      <c r="B89" s="27" t="str">
         <f t="shared" si="2"/>
         <v>LoaiThuChiController</v>
       </c>
-      <c r="C89" s="30" t="str">
+      <c r="C89" s="27" t="str">
         <f t="shared" si="3"/>
         <v>LoaiThuChi</v>
       </c>
@@ -17885,11 +18174,11 @@
       <c r="A90" s="9">
         <v>88</v>
       </c>
-      <c r="B90" s="30" t="str">
+      <c r="B90" s="27" t="str">
         <f t="shared" si="2"/>
         <v>TaiSanDonViController</v>
       </c>
-      <c r="C90" s="30" t="str">
+      <c r="C90" s="27" t="str">
         <f t="shared" si="3"/>
         <v>TaiSanDonVi</v>
       </c>
@@ -17904,11 +18193,11 @@
       <c r="A91" s="9">
         <v>89</v>
       </c>
-      <c r="B91" s="30" t="str">
+      <c r="B91" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ChiTietTaiSanDonViController</v>
       </c>
-      <c r="C91" s="30" t="str">
+      <c r="C91" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ChiTietTaiSanDonVi</v>
       </c>
@@ -17923,11 +18212,11 @@
       <c r="A92" s="9">
         <v>90</v>
       </c>
-      <c r="B92" s="30" t="str">
+      <c r="B92" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ChiTietThuChiController</v>
       </c>
-      <c r="C92" s="30" t="str">
+      <c r="C92" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ChiTietThuChi</v>
       </c>
@@ -17942,11 +18231,11 @@
       <c r="A93" s="9">
         <v>91</v>
       </c>
-      <c r="B93" s="30" t="str">
+      <c r="B93" s="27" t="str">
         <f t="shared" si="2"/>
         <v>ChiTieuTuyenSinhTheoNganhController</v>
       </c>
-      <c r="C93" s="30" t="str">
+      <c r="C93" s="27" t="str">
         <f t="shared" si="3"/>
         <v>ChiTieuTuyenSinhTheoNganh</v>
       </c>
@@ -17961,11 +18250,11 @@
       <c r="A94" s="9">
         <v>92</v>
       </c>
-      <c r="B94" s="30" t="str">
+      <c r="B94" s="27" t="str">
         <f t="shared" si="2"/>
         <v>DuLieuTrungTuyenController</v>
       </c>
-      <c r="C94" s="30" t="str">
+      <c r="C94" s="27" t="str">
         <f t="shared" si="3"/>
         <v>DuLieuTrungTuyen</v>
       </c>
@@ -17980,11 +18269,11 @@
       <c r="A95" s="9">
         <v>93</v>
       </c>
-      <c r="B95" s="30" t="str">
+      <c r="B95" s="27" t="str">
         <f t="shared" si="2"/>
         <v>DanhSachVanBangChungChiController</v>
       </c>
-      <c r="C95" s="30" t="str">
+      <c r="C95" s="27" t="str">
         <f t="shared" si="3"/>
         <v>DanhSachVanBangChungChi</v>
       </c>

</xml_diff>